<commit_message>
adding Corey's Test case edits
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
   <si>
     <t xml:space="preserve">Test Case ID</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Module to be tested</t>
   </si>
   <si>
-    <t xml:space="preserve">Basic functionality test. Test List menu and see if Lists display, can you also enter a all lists and view the items inside them? Now can you add lists, can you add items?</t>
+    <t xml:space="preserve">Add Lists</t>
   </si>
   <si>
     <t xml:space="preserve">Assumptions</t>
@@ -61,21 +61,86 @@
     <t xml:space="preserve">Result</t>
   </si>
   <si>
+    <t xml:space="preserve">PASS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-when viewing any list (
+- Can add new list without selecting or inputting a test color. 
+-when creating a new list, it is added to the set of lists properly (in terms of ascetics anyway)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">view items in a list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">However, when viewing the list, there are a bunch of “Hello there” multiple times. About half of which have corresponding boxes checked off and half that do not. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Items to a list:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when adding an item, it is displayed with the correct name. However, it appears as though the ‘priority’ marker has no functional significance (at the time this was tested)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#0004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deleting Lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When ever an item has been checked or unchecked it will not be deleted and an error is thrown.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#0006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding new List</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">When creating a new list, (initially checkbox is unchecked) and if one tries to delete it in this state they can. However if they try to check it off and then delete they will be thrown a white label error. Can add list with no name OR color. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> also, if you delete it, you get an error.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -97,19 +162,44 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,7 +236,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -155,19 +245,47 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -188,15 +306,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J60" activeCellId="0" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -262,18 +380,495 @@
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" s="7" customFormat="true" ht="30.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-    </row>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" s="7" customFormat="true" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" s="7" customFormat="true" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="9"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+    </row>
+    <row r="52" s="7" customFormat="true" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="9"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" s="7" customFormat="true" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="45">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -282,7 +877,43 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B9:H12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:H25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:H38"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:H51"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:H64"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>